<commit_message>
update cv for cesab
</commit_message>
<xml_diff>
--- a/cv-data.xlsx
+++ b/cv-data.xlsx
@@ -305,11 +305,11 @@
     <t xml:space="preserve">Modélisation statistique explicative, prédictive et descriptive de divers indicateurs entomologiques spatio-temporels du risque de transmission du paludisme (présence, abondance, résistance physiologique et comportementale des moustiques) à l'aide de données hétérogènes, multi-sources et multi-échelles et de modèles d'apprentissage automatique.</t>
   </si>
   <si>
-    <t xml:space="preserve">**Projet Global Tuna Atlas : Mise en œuvre d’entrepôts de données spatio-temporalisées sur
+    <t xml:space="preserve">**Projet Global Tuna Atlas : Génération de jeux de données globaux spatio-temporalisées sur
 les pêcheries thonières et services FAIR associés**</t>
   </si>
   <si>
-    <t xml:space="preserve">Développement et gestion de bases de données spatio-temporelles, développement de chaînes de traitements complexes dans le langage R (extraction-transformation-chargement-publication de données), développement de librairies R, description et catalogage de données.</t>
+    <t xml:space="preserve">Création de jeux de données spatio-temporels complexes à partir de données hétérogènes, développement de chaînes de traitements complexes dans le langage R (extraction-transformation-chargement-publication de données), développement de librairies R, description et catalogage de données selon les principes FAIR.</t>
   </si>
   <si>
     <t xml:space="preserve">Géomaticien (Volontaire de Service Civique)</t>
@@ -772,7 +772,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
@@ -900,7 +900,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.51"/>
@@ -1050,7 +1050,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="60.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.33"/>
@@ -1269,7 +1269,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.83"/>
   </cols>
@@ -1321,12 +1321,12 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="65.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.32"/>
@@ -1514,12 +1514,12 @@
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="65.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.32"/>
@@ -1684,16 +1684,16 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="65.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.32"/>
@@ -1917,7 +1917,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
@@ -2050,7 +2050,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
@@ -2169,12 +2169,12 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="65.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.32"/>
@@ -2334,12 +2334,12 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="65.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.32"/>
@@ -2526,7 +2526,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.5"/>

</xml_diff>